<commit_message>
2dsn: Seat.seat_last, excel import
</commit_message>
<xml_diff>
--- a/anwesende/room/tests/data/rooms1.xlsx
+++ b/anwesende/room/tests/data/rooms1.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20369"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\ws\gl\anwesende\anwesende\room\tests\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{766567E4-3D05-4ECA-9E09-796F98B06128}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="10728" windowHeight="19272"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="10730" windowHeight="19270" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -23,42 +24,8 @@
 </workbook>
 </file>
 
-<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <authors>
-    <author>Lutz Prechelt</author>
-  </authors>
-  <commentList>
-    <comment ref="E1" authorId="0" shapeId="0">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>Lutz Prechelt:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-All cells must have text format, not number format!</t>
-        </r>
-      </text>
-    </comment>
-  </commentList>
-</comments>
-</file>
-
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="12">
   <si>
     <t>organization</t>
   </si>
@@ -72,12 +39,6 @@
     <t>room</t>
   </si>
   <si>
-    <t>seat_min</t>
-  </si>
-  <si>
-    <t>seat_max</t>
-  </si>
-  <si>
     <t>fu-berlin.de</t>
   </si>
   <si>
@@ -91,13 +52,22 @@
   </si>
   <si>
     <t>K40</t>
+  </si>
+  <si>
+    <t>seat_last</t>
+  </si>
+  <si>
+    <t>r2s7</t>
+  </si>
+  <si>
+    <t>r2s3</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="4" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -112,19 +82,6 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="9"/>
-      <color indexed="81"/>
-      <name val="Tahoma"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="9"/>
-      <color indexed="81"/>
-      <name val="Tahoma"/>
-      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -430,23 +387,23 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F3"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:E3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+      <selection activeCell="F1" sqref="F1:F1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.90625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="14.33203125" style="1" customWidth="1"/>
-    <col min="2" max="2" width="11.88671875" style="1" customWidth="1"/>
-    <col min="3" max="3" width="10.88671875" style="1" customWidth="1"/>
+    <col min="1" max="1" width="14.36328125" style="1" customWidth="1"/>
+    <col min="2" max="2" width="11.90625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="10.90625" style="1" customWidth="1"/>
     <col min="4" max="4" width="6" style="1" customWidth="1"/>
-    <col min="5" max="16384" width="8.88671875" style="1"/>
+    <col min="5" max="16384" width="8.90625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -460,55 +417,45 @@
         <v>3</v>
       </c>
       <c r="E1" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A2" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="B2" s="1" t="s">
         <v>5</v>
       </c>
+      <c r="C2" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>10</v>
+      </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A2" s="1" t="s">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A3" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C3" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B2" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C2" s="1" t="s">
+      <c r="D3" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="D2" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="E2" s="1">
-        <v>1</v>
-      </c>
-      <c r="F2" s="1">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A3" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="E3" s="1">
-        <v>1</v>
-      </c>
-      <c r="F3" s="1">
-        <v>6</v>
+      <c r="E3" s="1" t="s">
+        <v>11</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
-  <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Excel, views, documentation: add row_dist, seat_dist
</commit_message>
<xml_diff>
--- a/anwesende/room/tests/data/rooms1.xlsx
+++ b/anwesende/room/tests/data/rooms1.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20369"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20375"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\ws\gl\anwesende\anwesende\room\tests\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{766567E4-3D05-4ECA-9E09-796F98B06128}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4596D6C9-F6FF-4B12-8D63-332085948B02}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="10730" windowHeight="19270" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="17">
   <si>
     <t>organization</t>
   </si>
@@ -61,6 +61,21 @@
   </si>
   <si>
     <t>r2s3</t>
+  </si>
+  <si>
+    <t>row_dist</t>
+  </si>
+  <si>
+    <t>seat_dist</t>
+  </si>
+  <si>
+    <t>1,1</t>
+  </si>
+  <si>
+    <t>0,6</t>
+  </si>
+  <si>
+    <t>1,5</t>
   </si>
 </sst>
 </file>
@@ -388,10 +403,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E3"/>
+  <dimension ref="A1:G3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F1" sqref="F1:F1048576"/>
+      <selection activeCell="E3" sqref="E3:F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.90625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -400,10 +415,12 @@
     <col min="2" max="2" width="11.90625" style="1" customWidth="1"/>
     <col min="3" max="3" width="10.90625" style="1" customWidth="1"/>
     <col min="4" max="4" width="6" style="1" customWidth="1"/>
-    <col min="5" max="16384" width="8.90625" style="1"/>
+    <col min="5" max="5" width="9.1796875" style="1" customWidth="1"/>
+    <col min="6" max="6" width="8.36328125" style="1" customWidth="1"/>
+    <col min="7" max="16384" width="8.90625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -417,10 +434,16 @@
         <v>3</v>
       </c>
       <c r="E1" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="G1" s="2" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
         <v>4</v>
       </c>
@@ -434,10 +457,16 @@
         <v>7</v>
       </c>
       <c r="E2" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="G2" s="1" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
         <v>4</v>
       </c>
@@ -451,6 +480,12 @@
         <v>8</v>
       </c>
       <c r="E3" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G3" s="1" t="s">
         <v>11</v>
       </c>
     </row>

</xml_diff>